<commit_message>
Added config file and updated MyAccountTest
</commit_message>
<xml_diff>
--- a/src/test/resources/InvalidCredentialForLogin.xlsx
+++ b/src/test/resources/InvalidCredentialForLogin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neelam Nagariya\git\AutomationAssignment\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10555E11-28EF-45D7-9693-5D8591EC956C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC20CC15-4B79-432A-97A3-46228A4DD8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>email</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>abc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> riti@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Password2 </t>
   </si>
 </sst>
 </file>
@@ -390,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -418,22 +412,14 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added config in src/test, MyAccountTest updated
</commit_message>
<xml_diff>
--- a/src/test/resources/InvalidCredentialForLogin.xlsx
+++ b/src/test/resources/InvalidCredentialForLogin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neelam Nagariya\git\AutomationAssignment\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC20CC15-4B79-432A-97A3-46228A4DD8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C446EFD-40E9-4120-99EA-F5C37930EEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>email</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>Password2</t>
+  </si>
+  <si>
+    <t>r iti@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> riti@gmail.com </t>
   </si>
 </sst>
 </file>
@@ -99,10 +108,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -384,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -423,6 +433,22 @@
         <v>123</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{92B38F20-D245-4BB6-89BD-A897147647FB}"/>

</xml_diff>